<commit_message>
updated figure 4 and associated uncertainty data
</commit_message>
<xml_diff>
--- a/data/LUC_uncertainty_AR6_reanalysis.xlsx
+++ b/data/LUC_uncertainty_AR6_reanalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iiasahub-my.sharepoint.com/personal/gidden_iiasa_ac_at/Documents/work/iiasa/papers/ar6_reanalysis/gidden_ar6_reanalysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="11_FDC23FED930929B7CCFA85720D906DC21F0C36BE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7C98B24-F1EA-426E-92BB-7EDDD3D31DCC}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="11_FDC23FED930929B7CCFA85720D906DC21F0C36BE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9B7703B-E712-4770-84FE-C267F1E3CAC7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fig1AB" sheetId="6" r:id="rId1"/>
@@ -152,19 +152,19 @@
     <t>1.5C</t>
   </si>
   <si>
-    <t>Direct</t>
-  </si>
-  <si>
-    <t>Indirect</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>2C</t>
   </si>
   <si>
     <t>Current Policies</t>
+  </si>
+  <si>
+    <t>Land CDR (Direct)</t>
+  </si>
+  <si>
+    <t>Indirect Removals</t>
+  </si>
+  <si>
+    <t>Total Land Removals</t>
   </si>
 </sst>
 </file>
@@ -492,13 +492,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -518,7 +518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -538,7 +538,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -558,7 +558,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -578,7 +578,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -598,7 +598,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -628,9 +628,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -650,7 +650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -670,7 +670,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -703,13 +703,13 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -726,7 +726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -743,7 +743,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -760,7 +760,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -790,9 +790,9 @@
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -809,7 +809,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -826,7 +826,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -843,7 +843,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -860,7 +860,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -886,18 +886,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -914,7 +914,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -922,7 +922,7 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D2">
         <v>1.5604922299999999</v>
@@ -931,7 +931,7 @@
         <v>0.56774961999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -939,7 +939,7 @@
         <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>0.14834576999999999</v>
@@ -948,7 +948,7 @@
         <v>0.56053664000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -956,7 +956,7 @@
         <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>1.69833977</v>
@@ -965,15 +965,15 @@
         <v>0.90163512000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D5">
         <v>0.69711175000000003</v>
@@ -982,15 +982,15 @@
         <v>0.29704567999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
         <v>43</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
       </c>
       <c r="D6">
         <v>0.68208025000000005</v>
@@ -999,15 +999,15 @@
         <v>0.56519748000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D7">
         <v>1.16159558</v>
@@ -1016,15 +1016,15 @@
         <v>0.67883236000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D8">
         <v>5.946017E-2</v>
@@ -1033,15 +1033,15 @@
         <v>0.20002136000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D9">
         <v>1.07305206</v>
@@ -1050,15 +1050,15 @@
         <v>0.53691670000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
         <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>42</v>
       </c>
       <c r="D10">
         <v>1.13636336</v>
@@ -1076,18 +1076,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D2">
         <v>2.9684987199999999</v>
@@ -1121,7 +1121,7 @@
         <v>1.03604439</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>-1.8990523500000001</v>
@@ -1138,7 +1138,7 @@
         <v>1.22766514</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>1.1366604499999999</v>
@@ -1155,15 +1155,15 @@
         <v>1.4733103999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D5">
         <v>1.47527908</v>
@@ -1172,15 +1172,15 @@
         <v>0.65471425000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
         <v>43</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
       </c>
       <c r="D6">
         <v>-0.51000217999999997</v>
@@ -1189,15 +1189,15 @@
         <v>1.1281576499999999</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D7">
         <v>1.1894153999999999</v>
@@ -1206,15 +1206,15 @@
         <v>1.2596775099999999</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D8">
         <v>-0.32881325</v>
@@ -1223,15 +1223,15 @@
         <v>0.36987946999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D9">
         <v>2.1645246</v>
@@ -1240,15 +1240,15 @@
         <v>1.25091675</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
         <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>42</v>
       </c>
       <c r="D10">
         <v>1.95556961</v>

</xml_diff>

<commit_message>
update figs 2 and 4 based on thomas' feedback
</commit_message>
<xml_diff>
--- a/data/LUC_uncertainty_AR6_reanalysis.xlsx
+++ b/data/LUC_uncertainty_AR6_reanalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iiasahub-my.sharepoint.com/personal/gidden_iiasa_ac_at/Documents/work/iiasa/papers/ar6_reanalysis/gidden_ar6_reanalysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="11_FDC23FED930929B7CCFA85720D906DC21F0C36BE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57B328FD-A186-4ACB-BA3A-E248A45791AC}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="11_FDC23FED930929B7CCFA85720D906DC21F0C36BE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{345EAB76-362C-4A81-970F-CC01E1D25B15}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fig1AB" sheetId="6" r:id="rId1"/>
@@ -140,9 +140,6 @@
     <t>2010-2020</t>
   </si>
   <si>
-    <t>BK/IAM</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>2012-2021</t>
+  </si>
+  <si>
+    <t>Model</t>
   </si>
 </sst>
 </file>
@@ -529,10 +529,10 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2">
         <v>2005</v>
@@ -549,10 +549,10 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3">
         <v>2015</v>
@@ -572,7 +572,7 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>2005</v>
@@ -592,7 +592,7 @@
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5">
         <v>2015</v>
@@ -908,10 +908,10 @@
         <v>20</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>19</v>
@@ -925,10 +925,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2">
         <v>1.5604922299999999</v>
@@ -942,10 +942,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3">
         <v>0.14834576999999999</v>
@@ -959,10 +959,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>1.69833977</v>
@@ -976,10 +976,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5">
         <v>0.69711175000000003</v>
@@ -993,10 +993,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6">
         <v>0.68208025000000005</v>
@@ -1010,10 +1010,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7">
         <v>1.16159558</v>
@@ -1027,10 +1027,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
         <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
       </c>
       <c r="D8">
         <v>5.946017E-2</v>
@@ -1044,10 +1044,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9">
         <v>1.07305206</v>
@@ -1061,10 +1061,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10">
         <v>1.13636336</v>
@@ -1098,10 +1098,10 @@
         <v>20</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>19</v>
@@ -1115,10 +1115,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2">
         <v>2.9684987199999999</v>
@@ -1132,10 +1132,10 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3">
         <v>-1.8990523500000001</v>
@@ -1149,10 +1149,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>1.1366604499999999</v>
@@ -1166,10 +1166,10 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5">
         <v>1.47527908</v>
@@ -1183,10 +1183,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6">
         <v>-0.51000217999999997</v>
@@ -1200,10 +1200,10 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7">
         <v>1.1894153999999999</v>
@@ -1217,10 +1217,10 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
         <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
       </c>
       <c r="D8">
         <v>-0.32881325</v>
@@ -1234,10 +1234,10 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9">
         <v>2.1645246</v>
@@ -1251,10 +1251,10 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10">
         <v>1.95556961</v>

</xml_diff>

<commit_message>
update figures for nature editor preferences
</commit_message>
<xml_diff>
--- a/data/LUC_uncertainty_AR6_reanalysis.xlsx
+++ b/data/LUC_uncertainty_AR6_reanalysis.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iiasahub-my.sharepoint.com/personal/gidden_iiasa_ac_at/Documents/work/iiasa/papers/ar6_reanalysis/gidden_ar6_reanalysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="11_FDC23FED930929B7CCFA85720D906DC21F0C36BE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{345EAB76-362C-4A81-970F-CC01E1D25B15}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="11_FDC23FED930929B7CCFA85720D906DC21F0C36BE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD41FE37-C3E4-450A-AFAD-684F6D29D117}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Fig1AB" sheetId="6" r:id="rId1"/>
+    <sheet name="Fig2AB" sheetId="6" r:id="rId1"/>
     <sheet name="extra_data" sheetId="7" r:id="rId2"/>
-    <sheet name="Fig1C" sheetId="4" r:id="rId3"/>
+    <sheet name="Fig2C" sheetId="4" r:id="rId3"/>
     <sheet name="extra_data_1C" sheetId="8" r:id="rId4"/>
     <sheet name="Fig4C" sheetId="1" r:id="rId5"/>
     <sheet name="Fig4D" sheetId="3" r:id="rId6"/>
@@ -494,7 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -705,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>